<commit_message>
work on multi controls
</commit_message>
<xml_diff>
--- a/storage/app/repository/mvsp-3.0.xlsx
+++ b/storage/app/repository/mvsp-3.0.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
+  <si>
+    <t xml:space="preserve">Framework</t>
+  </si>
   <si>
     <t xml:space="preserve">Domain</t>
   </si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Action Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVSP</t>
   </si>
   <si>
     <t xml:space="preserve">MVSP:BU</t>
@@ -760,134 +766,29 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="59.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="32.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="44.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="59.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,7 +798,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -906,7 +807,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -918,715 +819,793 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7"/>
       <c r="H2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="I2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="7"/>
       <c r="H6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="7"/>
       <c r="H9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="9"/>
+      <c r="F10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="F11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="7"/>
       <c r="H11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="F12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>72</v>
       </c>
+      <c r="F13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>77</v>
       </c>
+      <c r="F14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="F15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="7"/>
       <c r="H15" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="F16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="F17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="7"/>
       <c r="H17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>99</v>
       </c>
+      <c r="F18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>104</v>
       </c>
+      <c r="F19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="F20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="7"/>
       <c r="H20" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="9"/>
+        <v>111</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="E21" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="7"/>
       <c r="H21" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="E22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>124</v>
       </c>
+      <c r="F23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="7"/>
       <c r="H23" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="9"/>
+        <v>126</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>129</v>
       </c>
+      <c r="F24" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="7"/>
       <c r="H24" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="9"/>
+        <v>131</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>134</v>
       </c>
+      <c r="F25" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="7"/>
       <c r="H25" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="9"/>
+        <v>136</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>139</v>
       </c>
+      <c r="F26" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="7"/>
       <c r="H26" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="9"/>
+        <v>141</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>